<commit_message>
insumo prima cedida requiere fecha expedicion para cruzar con gasto
</commit_message>
<xml_diff>
--- a/prototipo_pcr/inputs/componente_pcr.xlsx
+++ b/prototipo_pcr/inputs/componente_pcr.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suramericana.sharepoint.com/sites/TraNIFF/Shared Documents/féniX/01 IFRS17/02 Entregables Procesos/05 Reservas/03 PCR CP/03 Tecnología/01 Prototipo/prototipo_pcr/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72CE9F21-9FFF-D445-B0AE-1D1799027CFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{72CE9F21-9FFF-D445-B0AE-1D1799027CFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{700D5A2D-AF43-794C-A3D2-3598072B4070}"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="2820" windowWidth="26440" windowHeight="15200" xr2:uid="{D5F5BCB5-C8DF-CB40-B9F9-75ACE26DF25B}"/>
+    <workbookView xWindow="2600" yWindow="2860" windowWidth="26440" windowHeight="15200" xr2:uid="{D5F5BCB5-C8DF-CB40-B9F9-75ACE26DF25B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
   <si>
     <t>componente</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>ajuste_dac_otros</t>
+  </si>
+  <si>
+    <t>camara_soat</t>
+  </si>
+  <si>
+    <t>CAM</t>
   </si>
 </sst>
 </file>
@@ -500,9 +506,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B32BF04-3379-8D40-9523-DB61E3824C24}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -663,6 +671,14 @@
       </c>
       <c r="C14" s="2" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -892,13 +908,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9B5B59D-333C-4E11-90C6-AF3EA23AA592}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F39AE822-39D7-4DA9-A569-FF676754C511}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43690494-4B82-49FC-BC39-E7631EE33B1B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82A82584-C4E2-4EA3-A59B-5B6C7C29DEC4}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97F04C1C-06CF-467A-ACC4-0CC94B466170}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21455BB0-279F-4E8C-AF4F-8AA2CAD4B63F}"/>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{3c0bd4fe-1111-4d13-8e0c-7c33b9eb7581}" enabled="0" method="" siteId="{3c0bd4fe-1111-4d13-8e0c-7c33b9eb7581}" removed="1"/>
+</clbl:labelList>
 </file>
</xml_diff>